<commit_message>
linked to learning about electronics
</commit_message>
<xml_diff>
--- a/assets/calculations/TransistorVibromotorCalculations.xlsx
+++ b/assets/calculations/TransistorVibromotorCalculations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\physcomp\assets\calculations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8966479E-71D6-4609-AAF4-80D604C0FB05}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BA81BB2-0B06-4627-9C6E-18550A6F04B1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5330" yWindow="4100" windowWidth="28800" windowHeight="15560" xr2:uid="{501760FD-0469-4BFC-B033-3A0BF35CF7E9}"/>
+    <workbookView xWindow="3860" yWindow="4120" windowWidth="28800" windowHeight="15560" xr2:uid="{501760FD-0469-4BFC-B033-3A0BF35CF7E9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="21">
   <si>
     <t>1K Resistor
 Transistor Control Input Current</t>
@@ -550,7 +550,7 @@
   <dimension ref="A1:U26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T23" sqref="T23"/>
+      <selection activeCell="K28" sqref="K28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>